<commit_message>
T4.1 re-run all data processing scripts
</commit_message>
<xml_diff>
--- a/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_vdReijden.xlsx
+++ b/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/DataExtractionForm_WP4_vdReijden.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://share.dtu.dk/sites/SEAwise_517900/Shared Documents/WP4 Ecological effects of fisheries/Task 4.1/Data extraction/Data extraction files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/estb_dtu_dk/Documents/Projects/SEAwise/SEAwise GitHub/Systematic Reviews/Analysis Task 4.1/Data_Extraction_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0306A68-4E8C-47EE-B297-9A19847CAC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{F0306A68-4E8C-47EE-B297-9A19847CAC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{017043E8-C8CF-4D80-AB1B-D60B3E9FE4F2}"/>
   <bookViews>
-    <workbookView xWindow="-4650" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataExtraction" sheetId="1" r:id="rId1"/>
@@ -6311,7 +6311,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Validation"/>
@@ -6324,17 +6324,13 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="DataExtraction"/>
       <sheetName val="Validation"/>
-      <sheetName val="Drop-down overview"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6603,45 +6599,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AX182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="AW94" sqref="AW94"/>
+      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="2.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" customWidth="1"/>
-    <col min="5" max="5" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
-    <col min="7" max="7" width="2.1796875" customWidth="1"/>
-    <col min="8" max="9" width="2.54296875" customWidth="1"/>
-    <col min="10" max="10" width="1.7265625" customWidth="1"/>
-    <col min="11" max="11" width="10.81640625" customWidth="1"/>
-    <col min="12" max="12" width="2.54296875" customWidth="1"/>
+    <col min="7" max="7" width="2.140625" customWidth="1"/>
+    <col min="8" max="9" width="2.5703125" customWidth="1"/>
+    <col min="10" max="10" width="1.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="2.5703125" customWidth="1"/>
     <col min="13" max="13" width="3" customWidth="1"/>
-    <col min="14" max="14" width="2.81640625" customWidth="1"/>
-    <col min="15" max="15" width="2.453125" customWidth="1"/>
-    <col min="16" max="16" width="2.81640625" customWidth="1"/>
-    <col min="17" max="17" width="8.7265625" customWidth="1"/>
-    <col min="19" max="19" width="18.1796875" customWidth="1"/>
-    <col min="24" max="25" width="32.7265625" customWidth="1"/>
-    <col min="34" max="35" width="17.7265625" customWidth="1"/>
-    <col min="36" max="36" width="18.7265625" customWidth="1"/>
-    <col min="37" max="37" width="19.1796875" customWidth="1"/>
-    <col min="38" max="38" width="17.7265625" customWidth="1"/>
-    <col min="39" max="39" width="14.26953125" customWidth="1"/>
-    <col min="40" max="41" width="15.81640625" customWidth="1"/>
-    <col min="42" max="42" width="15.453125" customWidth="1"/>
-    <col min="46" max="46" width="15.1796875" customWidth="1"/>
-    <col min="47" max="47" width="18.7265625" customWidth="1"/>
+    <col min="14" max="14" width="2.85546875" customWidth="1"/>
+    <col min="15" max="15" width="2.42578125" customWidth="1"/>
+    <col min="16" max="16" width="2.85546875" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" customWidth="1"/>
+    <col min="19" max="19" width="18.140625" customWidth="1"/>
+    <col min="24" max="25" width="32.7109375" customWidth="1"/>
+    <col min="34" max="35" width="17.7109375" customWidth="1"/>
+    <col min="36" max="36" width="18.7109375" customWidth="1"/>
+    <col min="37" max="37" width="19.140625" customWidth="1"/>
+    <col min="38" max="38" width="17.7109375" customWidth="1"/>
+    <col min="39" max="39" width="14.28515625" customWidth="1"/>
+    <col min="40" max="41" width="15.85546875" customWidth="1"/>
+    <col min="42" max="42" width="15.42578125" customWidth="1"/>
+    <col min="46" max="46" width="15.140625" customWidth="1"/>
+    <col min="47" max="47" width="18.7109375" customWidth="1"/>
     <col min="48" max="48" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
@@ -6707,7 +6704,7 @@
       <c r="AW1" s="11"/>
       <c r="AX1" s="11"/>
     </row>
-    <row r="2" spans="1:50" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:50" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
@@ -6859,7 +6856,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>242</v>
       </c>
@@ -6978,7 +6975,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>252</v>
       </c>
@@ -7022,7 +7019,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>257</v>
       </c>
@@ -7141,7 +7138,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>257</v>
       </c>
@@ -7260,7 +7257,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>257</v>
       </c>
@@ -7373,7 +7370,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>257</v>
       </c>
@@ -7486,7 +7483,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>257</v>
       </c>
@@ -7596,7 +7593,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>257</v>
       </c>
@@ -7706,7 +7703,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>263</v>
       </c>
@@ -7822,7 +7819,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>263</v>
       </c>
@@ -7944,7 +7941,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>269</v>
       </c>
@@ -7988,7 +7985,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>275</v>
       </c>
@@ -8101,7 +8098,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>275</v>
       </c>
@@ -8211,7 +8208,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>275</v>
       </c>
@@ -8324,7 +8321,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>281</v>
       </c>
@@ -8443,7 +8440,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>281</v>
       </c>
@@ -8562,7 +8559,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>287</v>
       </c>
@@ -8690,7 +8687,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>287</v>
       </c>
@@ -8821,7 +8818,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>293</v>
       </c>
@@ -8874,7 +8871,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>300</v>
       </c>
@@ -8993,7 +8990,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="23" spans="1:50" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:50" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>305</v>
       </c>
@@ -9115,7 +9112,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>311</v>
       </c>
@@ -9222,7 +9219,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>311</v>
       </c>
@@ -9338,7 +9335,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>311</v>
       </c>
@@ -9451,7 +9448,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>317</v>
       </c>
@@ -9576,7 +9573,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>317</v>
       </c>
@@ -9707,7 +9704,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>317</v>
       </c>
@@ -9829,7 +9826,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>317</v>
       </c>
@@ -9957,7 +9954,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>317</v>
       </c>
@@ -10082,7 +10079,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>317</v>
       </c>
@@ -10213,7 +10210,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>324</v>
       </c>
@@ -10329,7 +10326,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>329</v>
       </c>
@@ -10385,7 +10382,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="35" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>335</v>
       </c>
@@ -10516,7 +10513,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="36" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>335</v>
       </c>
@@ -10647,7 +10644,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="37" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>335</v>
       </c>
@@ -10778,7 +10775,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="38" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>340</v>
       </c>
@@ -10906,7 +10903,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="39" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>346</v>
       </c>
@@ -10950,7 +10947,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>351</v>
       </c>
@@ -11075,7 +11072,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>358</v>
       </c>
@@ -11200,7 +11197,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>358</v>
       </c>
@@ -11325,7 +11322,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="43" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>358</v>
       </c>
@@ -11450,7 +11447,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="44" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>363</v>
       </c>
@@ -11578,7 +11575,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="45" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>369</v>
       </c>
@@ -11709,7 +11706,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="46" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>376</v>
       </c>
@@ -11765,7 +11762,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="47" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>382</v>
       </c>
@@ -11902,7 +11899,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="48" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>388</v>
       </c>
@@ -11958,7 +11955,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>395</v>
       </c>
@@ -12086,7 +12083,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>401</v>
       </c>
@@ -12214,7 +12211,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="51" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>407</v>
       </c>
@@ -12345,7 +12342,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="52" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>413</v>
       </c>
@@ -12458,7 +12455,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="53" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>418</v>
       </c>
@@ -12583,7 +12580,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="54" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>425</v>
       </c>
@@ -12699,7 +12696,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="55" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>425</v>
       </c>
@@ -12827,7 +12824,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="56" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>425</v>
       </c>
@@ -12958,7 +12955,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="57" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>425</v>
       </c>
@@ -13089,7 +13086,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="58" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>431</v>
       </c>
@@ -13139,7 +13136,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>437</v>
       </c>
@@ -13192,7 +13189,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="60" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>443</v>
       </c>
@@ -13323,7 +13320,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="61" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>449</v>
       </c>
@@ -13448,7 +13445,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="62" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>449</v>
       </c>
@@ -13573,7 +13570,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="63" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>455</v>
       </c>
@@ -13698,7 +13695,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="64" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>455</v>
       </c>
@@ -13820,7 +13817,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="65" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>455</v>
       </c>
@@ -13948,7 +13945,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="66" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>460</v>
       </c>
@@ -14073,7 +14070,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="67" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>460</v>
       </c>
@@ -14198,7 +14195,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="68" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>460</v>
       </c>
@@ -14323,7 +14320,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="69" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>465</v>
       </c>
@@ -14451,7 +14448,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="70" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>465</v>
       </c>
@@ -14579,7 +14576,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="71" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>465</v>
       </c>
@@ -14710,7 +14707,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="72" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>471</v>
       </c>
@@ -14826,7 +14823,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="73" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>471</v>
       </c>
@@ -14948,7 +14945,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="74" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>477</v>
       </c>
@@ -15076,7 +15073,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="75" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>477</v>
       </c>
@@ -15204,7 +15201,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="76" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>477</v>
       </c>
@@ -15332,7 +15329,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="77" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>477</v>
       </c>
@@ -15460,7 +15457,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="78" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>483</v>
       </c>
@@ -15594,7 +15591,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="79" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>483</v>
       </c>
@@ -15728,7 +15725,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="80" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>488</v>
       </c>
@@ -15859,7 +15856,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="81" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>493</v>
       </c>
@@ -15975,7 +15972,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="82" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>493</v>
       </c>
@@ -16091,7 +16088,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="83" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>493</v>
       </c>
@@ -16207,7 +16204,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="84" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>499</v>
       </c>
@@ -16329,7 +16326,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="85" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>504</v>
       </c>
@@ -16451,7 +16448,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="86" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>509</v>
       </c>
@@ -16582,7 +16579,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="87" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>509</v>
       </c>
@@ -16710,7 +16707,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="88" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>514</v>
       </c>
@@ -16832,7 +16829,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="89" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>519</v>
       </c>
@@ -16957,7 +16954,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="90" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>525</v>
       </c>
@@ -17079,7 +17076,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="91" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>525</v>
       </c>
@@ -17201,7 +17198,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="92" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>525</v>
       </c>
@@ -17323,7 +17320,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="93" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>525</v>
       </c>
@@ -17445,7 +17442,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="94" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>531</v>
       </c>
@@ -17576,7 +17573,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="95" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>531</v>
       </c>
@@ -17707,7 +17704,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="96" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>538</v>
       </c>
@@ -17835,7 +17832,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="97" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>544</v>
       </c>
@@ -17963,7 +17960,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="98" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>549</v>
       </c>
@@ -18085,7 +18082,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="99" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>549</v>
       </c>
@@ -18207,7 +18204,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="100" spans="1:50" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:50" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>554</v>
       </c>
@@ -18323,7 +18320,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="101" spans="1:50" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:50" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>554</v>
       </c>
@@ -18442,7 +18439,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="102" spans="1:50" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:50" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>554</v>
       </c>
@@ -18561,7 +18558,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="103" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>559</v>
       </c>
@@ -18689,7 +18686,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="104" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>565</v>
       </c>
@@ -18811,7 +18808,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="105" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>565</v>
       </c>
@@ -18933,7 +18930,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="106" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>565</v>
       </c>
@@ -19052,7 +19049,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="107" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>570</v>
       </c>
@@ -19180,7 +19177,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="108" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>570</v>
       </c>
@@ -19308,7 +19305,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="109" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>570</v>
       </c>
@@ -19433,7 +19430,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="110" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>570</v>
       </c>
@@ -19561,7 +19558,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="111" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>575</v>
       </c>
@@ -19674,7 +19671,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="112" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>575</v>
       </c>
@@ -19790,7 +19787,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="113" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>575</v>
       </c>
@@ -19906,7 +19903,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="114" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>575</v>
       </c>
@@ -20022,7 +20019,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="115" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>581</v>
       </c>
@@ -20141,7 +20138,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="116" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>581</v>
       </c>
@@ -20260,7 +20257,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="117" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>581</v>
       </c>
@@ -20379,7 +20376,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="118" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>581</v>
       </c>
@@ -20498,7 +20495,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="119" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>581</v>
       </c>
@@ -20617,7 +20614,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="120" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>581</v>
       </c>
@@ -20736,7 +20733,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="121" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>587</v>
       </c>
@@ -20789,7 +20786,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="122" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>985</v>
       </c>
@@ -20917,7 +20914,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="123" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>979</v>
       </c>
@@ -21042,7 +21039,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="124" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>974</v>
       </c>
@@ -21167,7 +21164,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="125" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>968</v>
       </c>
@@ -21289,7 +21286,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="126" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>968</v>
       </c>
@@ -21411,7 +21408,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="127" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>968</v>
       </c>
@@ -21533,7 +21530,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="128" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>962</v>
       </c>
@@ -21658,7 +21655,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="129" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>962</v>
       </c>
@@ -21783,7 +21780,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="130" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>962</v>
       </c>
@@ -21908,7 +21905,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="131" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>962</v>
       </c>
@@ -22033,7 +22030,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="132" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>956</v>
       </c>
@@ -22089,7 +22086,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="133" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>951</v>
       </c>
@@ -22217,7 +22214,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="134" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>951</v>
       </c>
@@ -22345,7 +22342,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="135" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>951</v>
       </c>
@@ -22473,7 +22470,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="136" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>951</v>
       </c>
@@ -22601,7 +22598,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="137" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>946</v>
       </c>
@@ -22723,7 +22720,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="138" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>946</v>
       </c>
@@ -22845,7 +22842,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="139" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>941</v>
       </c>
@@ -22967,7 +22964,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="140" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>941</v>
       </c>
@@ -23092,7 +23089,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="141" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>936</v>
       </c>
@@ -23142,7 +23139,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="142" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>1030</v>
       </c>
@@ -23273,7 +23270,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="143" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>1030</v>
       </c>
@@ -23395,7 +23392,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="144" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>1035</v>
       </c>
@@ -23448,7 +23445,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="145" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>1041</v>
       </c>
@@ -23501,7 +23498,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="146" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>1047</v>
       </c>
@@ -23554,7 +23551,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="147" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>1052</v>
       </c>
@@ -23664,7 +23661,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="148" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>1057</v>
       </c>
@@ -23789,7 +23786,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="149" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>1057</v>
       </c>
@@ -23914,7 +23911,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="150" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>1062</v>
       </c>
@@ -23970,7 +23967,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="151" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>1068</v>
       </c>
@@ -24101,7 +24098,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="152" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>1068</v>
       </c>
@@ -24232,7 +24229,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="153" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>1068</v>
       </c>
@@ -24357,7 +24354,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="154" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>1075</v>
       </c>
@@ -24413,7 +24410,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="155" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>1106</v>
       </c>
@@ -24535,7 +24532,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="156" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>1106</v>
       </c>
@@ -24657,7 +24654,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="157" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>1106</v>
       </c>
@@ -24779,7 +24776,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="158" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>1106</v>
       </c>
@@ -24901,7 +24898,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="159" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>1106</v>
       </c>
@@ -25023,7 +25020,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="160" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>1106</v>
       </c>
@@ -25145,7 +25142,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="161" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>1106</v>
       </c>
@@ -25267,7 +25264,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="162" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>1106</v>
       </c>
@@ -25389,7 +25386,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="163" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>1106</v>
       </c>
@@ -25511,7 +25508,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="164" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>1106</v>
       </c>
@@ -25633,7 +25630,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="165" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>1111</v>
       </c>
@@ -25686,7 +25683,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="166" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>1117</v>
       </c>
@@ -25817,7 +25814,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="167" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>1117</v>
       </c>
@@ -25948,7 +25945,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="168" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>1117</v>
       </c>
@@ -26073,7 +26070,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="169" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>1117</v>
       </c>
@@ -26198,7 +26195,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="170" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>1122</v>
       </c>
@@ -26335,7 +26332,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="171" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>1122</v>
       </c>
@@ -26466,7 +26463,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="172" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>1127</v>
       </c>
@@ -26522,7 +26519,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="173" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>1133</v>
       </c>
@@ -26650,7 +26647,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="174" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>1133</v>
       </c>
@@ -26778,7 +26775,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="175" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>1133</v>
       </c>
@@ -26906,7 +26903,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="176" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>1133</v>
       </c>
@@ -27034,7 +27031,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="177" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>1133</v>
       </c>
@@ -27162,7 +27159,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="178" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>1138</v>
       </c>
@@ -27281,7 +27278,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="179" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>1138</v>
       </c>
@@ -27400,7 +27397,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="180" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>1143</v>
       </c>
@@ -27453,7 +27450,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="181" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>1148</v>
       </c>
@@ -27581,7 +27578,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="182" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:50" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>1153</v>
       </c>
@@ -27719,6 +27716,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:AX182" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="25">
+      <filters>
+        <filter val="NA"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="AQ1:AT1"/>
     <mergeCell ref="AU1:AX1"/>
@@ -27874,17 +27878,17 @@
       <selection activeCell="AG10" sqref="AG10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="32.1796875" customWidth="1"/>
-    <col min="23" max="23" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.140625" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="25" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="25" customWidth="1"/>
-    <col min="32" max="32" width="14.7265625" customWidth="1"/>
-    <col min="33" max="33" width="26.26953125" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+    <col min="33" max="33" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
@@ -27949,7 +27953,7 @@
       <c r="AV1" s="8"/>
       <c r="AW1" s="8"/>
     </row>
-    <row r="2" spans="1:49" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:49" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
@@ -28098,7 +28102,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="Q3" t="s">
         <v>21</v>
       </c>
@@ -28155,7 +28159,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="Q4" t="s">
         <v>22</v>
       </c>
@@ -28212,7 +28216,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="R5" t="s">
         <v>83</v>
       </c>
@@ -28268,7 +28272,7 @@
       </c>
       <c r="AW5" s="7"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:49" ht="30" x14ac:dyDescent="0.25">
       <c r="R6" t="s">
         <v>84</v>
       </c>
@@ -28313,7 +28317,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="R7" t="s">
         <v>85</v>
       </c>
@@ -28355,7 +28359,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="R8" t="s">
         <v>86</v>
       </c>
@@ -28393,7 +28397,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="R9" t="s">
         <v>87</v>
       </c>
@@ -28428,7 +28432,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="S10" t="s">
         <v>33</v>
       </c>
@@ -28463,7 +28467,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="S11" t="s">
         <v>32</v>
       </c>
@@ -28498,7 +28502,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="S12" t="s">
         <v>30</v>
       </c>
@@ -28530,7 +28534,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="S13" t="s">
         <v>79</v>
       </c>
@@ -28565,7 +28569,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="S14" t="s">
         <v>31</v>
       </c>
@@ -28594,7 +28598,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="S15" t="s">
         <v>35</v>
       </c>
@@ -28623,7 +28627,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="S16" t="s">
         <v>34</v>
       </c>
@@ -28643,7 +28647,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="17" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AM17" t="s">
         <v>165</v>
       </c>
@@ -28651,22 +28655,22 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="18" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AP18" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="19" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AP19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="22" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AH22" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="23" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AH23" s="6" t="s">
         <v>118</v>
       </c>
@@ -28701,7 +28705,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="24" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AH24" t="s">
         <v>132</v>
       </c>
@@ -28727,7 +28731,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="25" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AH25" t="s">
         <v>140</v>
       </c>
@@ -28750,7 +28754,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="26" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AJ26" t="s">
         <v>147</v>
       </c>
@@ -28761,7 +28765,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="27" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AJ27" t="s">
         <v>150</v>
       </c>
@@ -28772,7 +28776,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="28" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AJ28" t="s">
         <v>152</v>
       </c>
@@ -28780,12 +28784,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="29" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="29" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AP29" s="5" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="30" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AH30" s="5" t="s">
         <v>154</v>
       </c>
@@ -28808,7 +28812,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="31" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AH31" s="6" t="s">
         <v>132</v>
       </c>
@@ -28834,7 +28838,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="32" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AH32" t="s">
         <v>156</v>
       </c>
@@ -28860,7 +28864,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="33" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AH33" t="s">
         <v>158</v>
       </c>
@@ -28880,7 +28884,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="34" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AI34" t="s">
         <v>160</v>
       </c>
@@ -28894,7 +28898,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="35" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="35" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AI35" t="s">
         <v>116</v>
       </c>
@@ -28908,7 +28912,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="36" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AT36" t="s">
         <v>214</v>
       </c>
@@ -28916,10 +28920,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="37" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AL37" s="5"/>
     </row>
-    <row r="38" spans="34:47" x14ac:dyDescent="0.35">
+    <row r="38" spans="34:47" x14ac:dyDescent="0.25">
       <c r="AL38" s="6"/>
       <c r="AM38" s="6"/>
       <c r="AN38" s="6"/>
@@ -28947,37 +28951,37 @@
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.54296875" customWidth="1"/>
-    <col min="9" max="9" width="17.26953125" customWidth="1"/>
-    <col min="10" max="10" width="14.7265625" customWidth="1"/>
-    <col min="13" max="13" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
     <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.54296875" customWidth="1"/>
-    <col min="17" max="17" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.81640625" customWidth="1"/>
-    <col min="19" max="19" width="17.7265625" customWidth="1"/>
-    <col min="20" max="20" width="19.26953125" customWidth="1"/>
-    <col min="21" max="21" width="17.7265625" customWidth="1"/>
-    <col min="26" max="26" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5703125" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
+    <col min="20" max="20" width="19.28515625" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.453125" customWidth="1"/>
-    <col min="30" max="30" width="15.26953125" customWidth="1"/>
-    <col min="31" max="31" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.7265625" customWidth="1"/>
-    <col min="33" max="33" width="12.54296875" customWidth="1"/>
+    <col min="28" max="28" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" customWidth="1"/>
+    <col min="30" max="30" width="15.28515625" customWidth="1"/>
+    <col min="31" max="31" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+    <col min="33" max="33" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
@@ -29024,7 +29028,7 @@
       <c r="AF1" s="11"/>
       <c r="AG1" s="11"/>
     </row>
-    <row r="2" spans="1:33" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
@@ -29125,7 +29129,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -29187,7 +29191,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -29237,7 +29241,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -29290,7 +29294,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -29331,7 +29335,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -29375,7 +29379,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -29410,7 +29414,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -29445,7 +29449,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -29477,7 +29481,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>32</v>
       </c>
@@ -29506,7 +29510,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -29538,7 +29542,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>79</v>
       </c>
@@ -29567,7 +29571,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>31</v>
       </c>
@@ -29590,7 +29594,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>35</v>
       </c>
@@ -29616,7 +29620,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>34</v>
       </c>
@@ -29633,7 +29637,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="17" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q17" t="s">
         <v>122</v>
       </c>
@@ -29644,7 +29648,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="18" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="18" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q18" t="s">
         <v>123</v>
       </c>
@@ -29658,7 +29662,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="19" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R19" t="s">
         <v>155</v>
       </c>
@@ -29672,7 +29676,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="20" spans="17:28" x14ac:dyDescent="0.25">
       <c r="S20" t="s">
         <v>159</v>
       </c>
@@ -29683,7 +29687,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="21" spans="17:28" x14ac:dyDescent="0.25">
       <c r="S21" t="s">
         <v>231</v>
       </c>
@@ -29697,7 +29701,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="22" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="22" spans="17:28" x14ac:dyDescent="0.25">
       <c r="S22" t="s">
         <v>116</v>
       </c>
@@ -29708,7 +29712,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="23" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q23" t="s">
         <v>130</v>
       </c>
@@ -29719,7 +29723,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="24" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R24" t="s">
         <v>144</v>
       </c>
@@ -29727,7 +29731,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="25" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="25" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R25" t="s">
         <v>149</v>
       </c>
@@ -29735,7 +29739,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="26" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R26" t="s">
         <v>151</v>
       </c>
@@ -29743,7 +29747,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="27" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R27" t="s">
         <v>153</v>
       </c>
@@ -29757,7 +29761,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="28" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q28" t="s">
         <v>125</v>
       </c>
@@ -29768,7 +29772,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="29" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R29" t="s">
         <v>145</v>
       </c>
@@ -29779,7 +29783,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="30" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="30" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q30" t="s">
         <v>126</v>
       </c>
@@ -29790,7 +29794,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="31" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="31" spans="17:28" x14ac:dyDescent="0.25">
       <c r="R31" t="s">
         <v>146</v>
       </c>
@@ -29798,7 +29802,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="32" spans="17:28" x14ac:dyDescent="0.35">
+    <row r="32" spans="17:28" x14ac:dyDescent="0.25">
       <c r="Q32" t="s">
         <v>131</v>
       </c>
@@ -29806,12 +29810,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="26:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z33" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="34" spans="26:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="26:26" x14ac:dyDescent="0.25">
       <c r="Z34" t="s">
         <v>153</v>
       </c>
@@ -29831,6 +29835,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB0F5ECCA53DA47AEBDEAEE6167985F" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="125e2131eddd38cce17ebc9527d7a9d7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="553f2d8843fd2aa64b81f9e8c63a6619">
     <xsd:element name="properties">
@@ -29944,22 +29963,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C7BCA69-4CF2-4262-9455-76552C6346D5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29973,27 +30000,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{495201D0-9695-4A45-BC3A-28D949F46F55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66D459FE-C8DA-484C-BC8E-5EB6A351EBC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>